<commit_message>
Revert "Working dashboard (maybe)"
This reverts commit ecc70e1e13c86dafdaba0ef4fb8b6a3f83266806.
</commit_message>
<xml_diff>
--- a/data/CurrentLogDatasheet.xlsx
+++ b/data/CurrentLogDatasheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\App-Dev-2-Vargas\Diner-Ecommerce-Vargas-Project-main\mapua-lab-usage-and-monitoring\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOME\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F808C1E6-CD57-41E2-90F2-12A2FA157EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64EEE1A1-43B2-4F03-802B-BA3D76149D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15930" yWindow="1545" windowWidth="16305" windowHeight="11295" xr2:uid="{8C67381B-C88C-433D-AA1A-AD7533F48EDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{8C67381B-C88C-433D-AA1A-AD7533F48EDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -97,18 +98,6 @@
   </si>
   <si>
     <t>Time In</t>
-  </si>
-  <si>
-    <t>James, Rob</t>
-  </si>
-  <si>
-    <t>James, Roeid</t>
-  </si>
-  <si>
-    <t>Derby, Pretty</t>
-  </si>
-  <si>
-    <t>Umamusume, Jane</t>
   </si>
 </sst>
 </file>
@@ -461,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D133E5EB-D9A6-4194-BE38-71DD976F7569}">
-  <dimension ref="C2:G16"/>
+  <dimension ref="C2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,74 +653,6 @@
         <v>0.38819444444444445</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>2029864221</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.42986111111111114</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>2029864921</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.47152777777777777</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>2029855521</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.60763888888888884</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>2029888521</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.4909722222222222</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>